<commit_message>
modified:   construction_jobs.csv 	modified:   construction_jobs.xlsx 	modified:   plots/box_plot_closing_dates_by_sector.png 	modified:   plots/closing_date_frequency.png 	modified:   plots/company_distribution.png 	modified:   plots/correlation_matrix.png 	modified:   plots/facet_grid_job_distribution_by_company.png 	modified:   plots/heatmap_job_counts.png 	modified:   plots/job_titles_distribution.png 	modified:   plots/pair_grid_relationships.png 	modified:   plots/predictive_analysis_closing_date_vs_title_length.png 	modified:   plots/scatter_plot_title_length_vs_closing_date.png 	modified:   plots/title_length_distribution.png 	modified:   plots/trend_analysis_closing_dates_over_time.png 	modified:   plots/violin_plot_title_length_by_sector.png 	modified:   plots/word_cloud_job_titles.png 	modified:   scrape_log.csv
</commit_message>
<xml_diff>
--- a/construction_jobs.xlsx
+++ b/construction_jobs.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mason</t>
+          <t>Site Agent/Technician</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NS CONSTRUCTION LTD</t>
+          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>24/08/2024</t>
+          <t>29/08/2024</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mason</t>
+          <t>Site Engineer</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,7 +515,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>DATANG ENGINEERING CO LTD</t>
+          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>24/08/2024</t>
+          <t>29/08/2024</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Steel Fixer</t>
+          <t>Trainee Engineer</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>DATANG ENGINEERING CO LTD</t>
+          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>24/08/2024</t>
+          <t>29/08/2024</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Carpenter</t>
+          <t>Chief Supervisor</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -579,7 +579,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>DATANG ENGINEERING CO LTD</t>
+          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -589,7 +589,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>24/08/2024</t>
+          <t>29/08/2024</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Driver, Heavy Vehicle</t>
+          <t>Site Clerk</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>DATANG ENGINEERING CO LTD</t>
+          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>25/08/2024</t>
+          <t>29/08/2024</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Electrician</t>
+          <t>M &amp; E Coordinator</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DATANG ENGINEERING CO LTD</t>
+          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>25/08/2024</t>
+          <t>29/08/2024</t>
         </is>
       </c>
     </row>
@@ -665,7 +665,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Plumber</t>
+          <t>Handyman, Building Maintenance</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>DATANG ENGINEERING CO LTD</t>
+          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>25/08/2024</t>
+          <t>29/08/2024</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mason</t>
+          <t>Carpenter</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -707,7 +707,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>EASTERN ENGINEERING LTD</t>
+          <t>ECO DECK LTD</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>25/08/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Site Agent/Technician</t>
+          <t>Administrative Secretary</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -739,7 +739,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
+          <t>OPP CONTRACTING LTD</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>29/08/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Site Engineer</t>
+          <t>Administrative Officer</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
+          <t>OPP CONTRACTING LTD</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>29/08/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
     </row>
@@ -793,7 +793,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Trainee Engineer</t>
+          <t>General Worker</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>29/08/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Chief Supervisor</t>
+          <t>Plumber and Pipe Fitter, General</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -845,7 +845,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>29/08/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
     </row>
@@ -857,7 +857,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Site Clerk</t>
+          <t>Electrician</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>29/08/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
     </row>
@@ -889,7 +889,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>M &amp; E Coordinator</t>
+          <t>Site Supervisor</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
+          <t>OPP CONTRACTING LTD</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>29/08/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Handyman, Building Maintenance</t>
+          <t>Draughtsperson</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
+          <t>OPP CONTRACTING LTD</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>29/08/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
     </row>
@@ -953,7 +953,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Administrative Secretary</t>
+          <t>Purchasing Clerk</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Administrative Officer</t>
+          <t>Gardener</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -995,7 +995,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>OPP CONTRACTING LTD</t>
+          <t>RENOVATIA LTD</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>General Worker</t>
+          <t>Driver, Truck/Goods Vehicle/Chauffeur Poid-Lourd</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
+          <t>S M S CONTRACTING LTD</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
+          <t>SOLVCON LIMITED</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>31/08/2024</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Electrician</t>
+          <t>Accountant</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
+          <t>METASIGN COMPANY LTD</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>31/08/2024</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Site Supervisor</t>
+          <t>Welder</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>OPP CONTRACTING LTD</t>
+          <t>ECO DECK LTD</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>31/08/2024</t>
         </is>
       </c>
     </row>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Draughtsperson</t>
+          <t>Cabinet Maker/Menuisier</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>OPP CONTRACTING LTD</t>
+          <t>RBRB CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>31/08/2024</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Purchasing Clerk</t>
+          <t>Painter</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>OPP CONTRACTING LTD</t>
+          <t>RBRB CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>31/08/2024</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Gardener</t>
+          <t>Secretary</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>RENOVATIA LTD</t>
+          <t>PRO-DESIGN ENGINEERING CONSULTANTS LTD</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>31/08/2024</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Driver, Truck/Goods Vehicle/Chauffeur Poid-Lourd</t>
+          <t>Factory Operator</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>S M S CONTRACTING LTD</t>
+          <t>ECO DECK LTD</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>31/08/2024</t>
         </is>
       </c>
     </row>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Plumber and Pipe Fitter, General</t>
+          <t>Storekeeper</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>SOLVCON LIMITED</t>
+          <t>METASIGN COMPANY LTD</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Accountant</t>
+          <t>Receptionist</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>METASIGN COMPANY LTD</t>
+          <t>PRO-DESIGN ENGINEERING CONSULTANTS LTD</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1337,7 +1337,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Cabinet Maker/Menuisier</t>
+          <t>Administrative Clerk</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>RBRB CONSTRUCTION LTD</t>
+          <t>METASIGN COMPANY LTD</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Painter</t>
+          <t>Accounts clerk</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>RBRB CONSTRUCTION LTD</t>
+          <t>TOPBUILDER CO LTD</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Secretary</t>
+          <t>Procurement/Purchasing Officer</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>PRO-DESIGN ENGINEERING CONSULTANTS LTD</t>
+          <t>TOPBUILDER CO LTD</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Storekeeper</t>
+          <t>Electrical Technician</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>METASIGN COMPANY LTD</t>
+          <t>PROELEC ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Receptionist</t>
+          <t>Human Resource Officer</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>PRO-DESIGN ENGINEERING CONSULTANTS LTD</t>
+          <t>GREEN SCAFF CO LTD</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Administrative Clerk</t>
+          <t>Human Resource Assistant</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>METASIGN COMPANY LTD</t>
+          <t>SAFETY CONSTRUCTION CO LTD</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Accounts clerk</t>
+          <t>Engineer, Building Construction</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>TOPBUILDER CO LTD</t>
+          <t>JIANGXI CONSTRUCTION INTERNATIONAL ENGINEERING (MAURITIUS) CO LTD</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Procurement/Purchasing Officer</t>
+          <t>Technician, General</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>TOPBUILDER CO LTD</t>
+          <t>JIANGXI CONSTRUCTION INTERNATIONAL ENGINEERING (MAURITIUS) CO LTD</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Electrical Technician</t>
+          <t>Civil Engineer</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>PROELEC ELECTRICAL LTD</t>
+          <t>METASIGN COMPANY LTD</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Human Resource Officer</t>
+          <t>Site Supervisor</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1635,7 +1635,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>GREEN SCAFF CO LTD</t>
+          <t>METASIGN COMPANY LTD</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Human Resource Assistant</t>
+          <t>Electrician</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>SAFETY CONSTRUCTION CO LTD</t>
+          <t>PROELEC ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>31/08/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Engineer, Building Construction</t>
+          <t>Supervisor, Plumbing and Pipe Fitting</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>JIANGXI CONSTRUCTION INTERNATIONAL ENGINEERING (MAURITIUS) CO LTD</t>
+          <t>AKGM CONTRACTING LTD</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>31/08/2024</t>
+          <t>10/09/2024</t>
         </is>
       </c>
     </row>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Technician, General</t>
+          <t>Plumber and Pipe Fitter, General</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>JIANGXI CONSTRUCTION INTERNATIONAL ENGINEERING (MAURITIUS) CO LTD</t>
+          <t>AKGM CONTRACTING LTD</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>31/08/2024</t>
+          <t>10/09/2024</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Civil Engineer</t>
+          <t>Human Resource Assistant</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>METASIGN COMPANY LTD</t>
+          <t>AKGM CONTRACTING LTD</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>31/08/2024</t>
+          <t>12/09/2024</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Site Supervisor</t>
+          <t>M&amp;E Engineer</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>METASIGN COMPANY LTD</t>
+          <t>CIVELMEC GROUP LTD</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>31/08/2024</t>
+          <t>13/09/2024</t>
         </is>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Supervisor, Plumbing and Pipe Fitting</t>
+          <t>Cleaner, Building/Office</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>AKGM CONTRACTING LTD</t>
+          <t>ARWAN ENTERPRISE LTD</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>10/09/2024</t>
+          <t>20/09/2024</t>
         </is>
       </c>
     </row>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Plumber and Pipe Fitter, General</t>
+          <t>Accounts clerk</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>AKGM CONTRACTING LTD</t>
+          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>10/09/2024</t>
+          <t>20/09/2024</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Accounts clerk</t>
+          <t>Store Clerk</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>KUROS CONSTRUCTION SOLUTIONS LTD.</t>
+          <t>PROSEC LTD</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>20/09/2024</t>
+          <t>30/09/2024</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>M&amp;E Engineer</t>
+          <t>Administrative Clerk</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>CIVELMEC GROUP LTD</t>
+          <t>PROSEC LTD</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">

</xml_diff>